<commit_message>
changes to n2o quantification (needs revision)
</commit_message>
<xml_diff>
--- a/data/exp_raw/johann_batch_preprocessed.xlsx
+++ b/data/exp_raw/johann_batch_preprocessed.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="40">
   <si>
     <t>Name</t>
   </si>
@@ -149,6 +149,9 @@
   <si>
     <t>t</t>
   </si>
+  <si>
+    <t>dry weight (g)</t>
+  </si>
 </sst>
 </file>
 
@@ -157,7 +160,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,6 +192,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -198,7 +208,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -249,11 +259,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -329,9 +351,16 @@
     <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -609,15 +638,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S20" sqref="S20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -633,8 +662,11 @@
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F1" s="28" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -648,8 +680,11 @@
       <c r="E2" s="5">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F2" s="27">
+        <v>12.135000000000019</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -663,8 +698,11 @@
       <c r="E3" s="5">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F3" s="27">
+        <v>22.545000000000016</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
@@ -678,8 +716,11 @@
       <c r="E4" s="5">
         <v>2.9</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F4" s="27">
+        <v>12.605000000000018</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
@@ -693,8 +734,11 @@
       <c r="E5" s="5">
         <v>2.06</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F5" s="27">
+        <v>13.975000000000023</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
@@ -708,8 +752,11 @@
       <c r="E6" s="5">
         <v>40.1</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F6" s="27">
+        <v>5.1450000000000244</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>15</v>
       </c>
@@ -723,8 +770,11 @@
       <c r="E7" s="5">
         <v>24.6</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F7" s="27">
+        <v>5.5650000000000261</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>17</v>
       </c>
@@ -738,8 +788,11 @@
       <c r="E8" s="5">
         <v>0.89</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F8" s="27">
+        <v>17.325000000000017</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>19</v>
       </c>
@@ -753,8 +806,11 @@
       <c r="E9" s="5">
         <v>0.53</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F9" s="27">
+        <v>19.115000000000023</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
@@ -768,8 +824,11 @@
       <c r="E10" s="5">
         <v>3.49</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F10" s="27">
+        <v>13.135000000000019</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>21</v>
       </c>
@@ -783,8 +842,11 @@
       <c r="E11" s="5">
         <v>29.5</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F11" s="27">
+        <v>3.8150000000000261</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>22</v>
       </c>
@@ -798,8 +860,11 @@
       <c r="E12" s="5">
         <v>0.45</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F12" s="27">
+        <v>20.995000000000019</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>23</v>
       </c>
@@ -813,8 +878,11 @@
       <c r="E13" s="5">
         <v>19.600000000000001</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F13" s="27">
+        <v>3.3450000000000131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>25</v>
       </c>
@@ -828,8 +896,11 @@
       <c r="E14" s="5">
         <v>20.100000000000001</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F14" s="27">
+        <v>7.0950000000000131</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>26</v>
       </c>
@@ -843,8 +914,11 @@
       <c r="E15" s="5">
         <v>30.8</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F15" s="27">
+        <v>3.555000000000021</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>27</v>
       </c>
@@ -858,8 +932,11 @@
       <c r="E16" s="5">
         <v>4.9000000000000004</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F16" s="27">
+        <v>13.625000000000014</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>28</v>
       </c>
@@ -873,8 +950,11 @@
       <c r="E17" s="5">
         <v>25.4</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F17" s="27">
+        <v>5.7650000000000148</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>30</v>
       </c>
@@ -888,8 +968,11 @@
       <c r="E18" s="5">
         <v>11.2</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F18" s="27">
+        <v>5.8750000000000142</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>31</v>
       </c>
@@ -903,8 +986,11 @@
       <c r="E19" s="5">
         <v>8.5</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F19" s="27">
+        <v>8.9750000000000227</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>32</v>
       </c>
@@ -918,8 +1004,11 @@
       <c r="E20" s="5">
         <v>15.4</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F20" s="27">
+        <v>4.9350000000000165</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>33</v>
       </c>
@@ -933,8 +1022,11 @@
       <c r="E21" s="5">
         <v>9.4</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F21" s="27">
+        <v>6.2650000000000148</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>34</v>
       </c>
@@ -948,8 +1040,11 @@
       <c r="E22" s="5">
         <v>6.5</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F22" s="27">
+        <v>7.285000000000025</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>35</v>
       </c>
@@ -963,8 +1058,11 @@
       <c r="E23" s="5">
         <v>9.1</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F23" s="27">
+        <v>12.185000000000016</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>36</v>
       </c>
@@ -978,8 +1076,11 @@
       <c r="E24" s="5">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F24" s="27">
+        <v>15.115000000000023</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>37</v>
       </c>
@@ -992,6 +1093,9 @@
       </c>
       <c r="E25" s="5">
         <v>30.5</v>
+      </c>
+      <c r="F25" s="27">
+        <v>1.4750000000000227</v>
       </c>
     </row>
   </sheetData>
@@ -2459,7 +2563,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -5538,7 +5642,7 @@
   <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="K8" sqref="A8:K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update correction to sample weight in the database
</commit_message>
<xml_diff>
--- a/data/exp_raw/johann_batch_preprocessed.xlsx
+++ b/data/exp_raw/johann_batch_preprocessed.xlsx
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>Short ID</t>
-  </si>
-  <si>
-    <t>Fazies</t>
   </si>
   <si>
     <t>TOC %</t>
@@ -151,6 +148,9 @@
   </si>
   <si>
     <t>dry weight (g)</t>
+  </si>
+  <si>
+    <t>Facies</t>
   </si>
 </sst>
 </file>
@@ -641,14 +641,14 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -657,25 +657,25 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
       <c r="F1" s="28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="2">
         <v>23</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E2" s="5">
         <v>1.3</v>
@@ -686,14 +686,14 @@
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="2">
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="5">
         <v>0.65</v>
@@ -704,14 +704,14 @@
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="2">
         <v>4</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" s="5">
         <v>2.9</v>
@@ -722,14 +722,14 @@
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="2">
         <v>7</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" s="5">
         <v>2.06</v>
@@ -740,14 +740,14 @@
     </row>
     <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="2">
         <v>21</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E6" s="5">
         <v>40.1</v>
@@ -758,14 +758,14 @@
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="2">
         <v>17</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7" s="5">
         <v>24.6</v>
@@ -776,14 +776,14 @@
     </row>
     <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="2">
         <v>24</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E8" s="5">
         <v>0.89</v>
@@ -794,14 +794,14 @@
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="2">
         <v>3</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E9" s="5">
         <v>0.53</v>
@@ -812,14 +812,14 @@
     </row>
     <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="2">
         <v>9</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E10" s="5">
         <v>3.49</v>
@@ -830,14 +830,14 @@
     </row>
     <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="2">
         <v>22</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E11" s="5">
         <v>29.5</v>
@@ -848,14 +848,14 @@
     </row>
     <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="2">
         <v>1</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E12" s="5">
         <v>0.45</v>
@@ -866,14 +866,14 @@
     </row>
     <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="2">
         <v>11</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E13" s="5">
         <v>19.600000000000001</v>
@@ -884,14 +884,14 @@
     </row>
     <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="2">
         <v>18</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E14" s="5">
         <v>20.100000000000001</v>
@@ -902,14 +902,14 @@
     </row>
     <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="2">
         <v>20</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E15" s="5">
         <v>30.8</v>
@@ -920,14 +920,14 @@
     </row>
     <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="2">
         <v>6</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E16" s="5">
         <v>4.9000000000000004</v>
@@ -938,14 +938,14 @@
     </row>
     <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="2">
         <v>15</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E17" s="5">
         <v>25.4</v>
@@ -956,14 +956,14 @@
     </row>
     <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="2">
         <v>12</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E18" s="5">
         <v>11.2</v>
@@ -974,14 +974,14 @@
     </row>
     <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="2">
         <v>13</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E19" s="5">
         <v>8.5</v>
@@ -992,14 +992,14 @@
     </row>
     <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="2">
         <v>14</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E20" s="5">
         <v>15.4</v>
@@ -1010,14 +1010,14 @@
     </row>
     <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="2">
         <v>16</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E21" s="5">
         <v>9.4</v>
@@ -1028,14 +1028,14 @@
     </row>
     <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="2">
         <v>8</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E22" s="5">
         <v>6.5</v>
@@ -1046,14 +1046,14 @@
     </row>
     <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="2">
         <v>10</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E23" s="5">
         <v>9.1</v>
@@ -1064,14 +1064,14 @@
     </row>
     <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="2">
         <v>5</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E24" s="5">
         <v>3.4</v>
@@ -1082,14 +1082,14 @@
     </row>
     <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="2">
         <v>19</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E25" s="5">
         <v>30.5</v>
@@ -1115,7 +1115,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -1205,7 +1205,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="6">
         <f>34.941*5</f>
@@ -1263,7 +1263,7 @@
     </row>
     <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="6">
         <f>30.3*5</f>
@@ -1320,7 +1320,7 @@
     </row>
     <row r="3" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="6">
         <f>38.168*5</f>
@@ -1378,7 +1378,7 @@
     </row>
     <row r="4" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="6">
         <f>38.051*5</f>
@@ -1435,7 +1435,7 @@
     </row>
     <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="6">
         <f>37.342*5</f>
@@ -1491,7 +1491,7 @@
     </row>
     <row r="6" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="6">
         <f>37.054*5</f>
@@ -1545,7 +1545,7 @@
     </row>
     <row r="7" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="6">
         <f>14.738*5</f>
@@ -1599,7 +1599,7 @@
     </row>
     <row r="8" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="6">
         <f>39.99*5</f>
@@ -1653,7 +1653,7 @@
     </row>
     <row r="9" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="6">
         <f>39.473*5</f>
@@ -1711,7 +1711,7 @@
     </row>
     <row r="10" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="6">
         <f>40.286*5</f>
@@ -1766,7 +1766,7 @@
     </row>
     <row r="11" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="6">
         <f>32.395*5</f>
@@ -1823,7 +1823,7 @@
     </row>
     <row r="12" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="6">
         <f>39.738*5</f>
@@ -1879,7 +1879,7 @@
     </row>
     <row r="13" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" s="6">
         <f>38.163*5</f>
@@ -1935,7 +1935,7 @@
     </row>
     <row r="14" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="6">
         <f>38.477*5</f>
@@ -1991,7 +1991,7 @@
     </row>
     <row r="15" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" s="6">
         <f>37.926*5</f>
@@ -2049,7 +2049,7 @@
     </row>
     <row r="16" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" s="6">
         <f>40.787*5</f>
@@ -2104,7 +2104,7 @@
     </row>
     <row r="17" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" s="6">
         <f>41.464*5</f>
@@ -2159,7 +2159,7 @@
     </row>
     <row r="18" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18" s="6">
         <f>35.706*5</f>
@@ -2216,7 +2216,7 @@
     </row>
     <row r="19" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B19" s="6">
         <f>42.273*5</f>
@@ -2272,7 +2272,7 @@
     </row>
     <row r="20" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B20" s="6">
         <f>34.658*5</f>
@@ -2330,7 +2330,7 @@
     </row>
     <row r="21" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B21" s="6">
         <f>36.36*5</f>
@@ -2388,7 +2388,7 @@
     </row>
     <row r="22" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B22" s="6">
         <f>38.79*5</f>
@@ -2444,7 +2444,7 @@
     </row>
     <row r="23" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B23" s="6">
         <f>35.355*5</f>
@@ -2502,7 +2502,7 @@
     </row>
     <row r="24" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24" s="6">
         <f>36.304*5</f>
@@ -2571,7 +2571,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="9">
         <v>10.024394707585699</v>
@@ -2614,7 +2614,7 @@
     </row>
     <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="9">
         <v>11.3410595546338</v>
@@ -2657,7 +2657,7 @@
     </row>
     <row r="3" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="9">
         <v>8.0086674868742502</v>
@@ -2700,7 +2700,7 @@
     </row>
     <row r="4" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="9">
         <v>8.3092095523029599</v>
@@ -2743,7 +2743,7 @@
     </row>
     <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="9">
         <v>16.277277413358998</v>
@@ -2788,7 +2788,7 @@
     </row>
     <row r="6" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="9">
         <v>13.9971784435131</v>
@@ -2835,7 +2835,7 @@
     </row>
     <row r="7" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="9">
         <v>19.358082344819699</v>
@@ -2878,7 +2878,7 @@
     </row>
     <row r="8" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="9">
         <v>18.244566691448298</v>
@@ -2921,7 +2921,7 @@
     </row>
     <row r="9" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="9">
         <v>11.9934117263725</v>
@@ -2964,7 +2964,7 @@
     </row>
     <row r="10" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="9">
         <v>17.778009134467801</v>
@@ -3011,7 +3011,7 @@
     </row>
     <row r="11" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="9">
         <v>12.369356966486301</v>
@@ -3054,7 +3054,7 @@
     </row>
     <row r="12" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="9">
         <v>9.6149539395690695</v>
@@ -3097,7 +3097,7 @@
     </row>
     <row r="13" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" s="9">
         <v>13.2947818118211</v>
@@ -3142,7 +3142,7 @@
     </row>
     <row r="14" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="9">
         <v>17</v>
@@ -3187,7 +3187,7 @@
     </row>
     <row r="15" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" s="9">
         <v>7.7937454968791302</v>
@@ -3230,7 +3230,7 @@
     </row>
     <row r="16" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" s="9">
         <v>11.4698108577777</v>
@@ -3275,7 +3275,7 @@
     </row>
     <row r="17" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" s="9">
         <v>18</v>
@@ -3320,7 +3320,7 @@
     </row>
     <row r="18" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18" s="9">
         <v>13.499792796299801</v>
@@ -3365,7 +3365,7 @@
     </row>
     <row r="19" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B19" s="9">
         <v>21.1</v>
@@ -3410,7 +3410,7 @@
     </row>
     <row r="20" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B20" s="9">
         <v>11.8842377180758</v>
@@ -3455,7 +3455,7 @@
     </row>
     <row r="21" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B21" s="9">
         <v>10.144427996618001</v>
@@ -3498,7 +3498,7 @@
     </row>
     <row r="22" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B22" s="9">
         <v>18.585580659204801</v>
@@ -3543,7 +3543,7 @@
     </row>
     <row r="23" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B23" s="9">
         <v>10.004572696552801</v>
@@ -3586,7 +3586,7 @@
     </row>
     <row r="24" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24" s="9">
         <v>27.2917808308272</v>
@@ -3638,7 +3638,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="7">
         <v>20</v>
@@ -3679,7 +3679,7 @@
     </row>
     <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="12">
         <f>5.97*5</f>
@@ -3722,7 +3722,7 @@
     </row>
     <row r="3" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="12">
         <f>6.49*5</f>
@@ -3765,7 +3765,7 @@
     </row>
     <row r="4" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="12">
         <f>5.37*5</f>
@@ -3808,7 +3808,7 @@
     </row>
     <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="12">
         <f>4.71*5</f>
@@ -3851,7 +3851,7 @@
     </row>
     <row r="6" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="12">
         <f>4.22*5</f>
@@ -3893,7 +3893,7 @@
     </row>
     <row r="7" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="12">
         <f>5.83*5</f>
@@ -3932,7 +3932,7 @@
     </row>
     <row r="8" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="12">
         <f>3.83*5</f>
@@ -3974,7 +3974,7 @@
     </row>
     <row r="9" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="12">
         <f>5.72*5</f>
@@ -4016,7 +4016,7 @@
     </row>
     <row r="10" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="12">
         <f>6.14*5</f>
@@ -4057,7 +4057,7 @@
     </row>
     <row r="11" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="12">
         <f>12.64*5</f>
@@ -4100,7 +4100,7 @@
     </row>
     <row r="12" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="12">
         <f>6.95*5</f>
@@ -4143,7 +4143,7 @@
     </row>
     <row r="13" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" s="15">
         <f>5.842*5</f>
@@ -4185,7 +4185,7 @@
     </row>
     <row r="14" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="15">
         <f>3.738*5</f>
@@ -4227,7 +4227,7 @@
     </row>
     <row r="15" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" s="15">
         <f>3.712*5</f>
@@ -4269,7 +4269,7 @@
     </row>
     <row r="16" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" s="15">
         <f>5.695*5</f>
@@ -4311,7 +4311,7 @@
     </row>
     <row r="17" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" s="15">
         <f>8.065*5</f>
@@ -4353,7 +4353,7 @@
     </row>
     <row r="18" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18" s="15">
         <f>6.307*5</f>
@@ -4395,7 +4395,7 @@
     </row>
     <row r="19" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B19" s="15">
         <f>6.446*5</f>
@@ -4435,7 +4435,7 @@
     </row>
     <row r="20" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B20" s="15">
         <f>4.356*5</f>
@@ -4476,7 +4476,7 @@
     </row>
     <row r="21" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B21" s="7">
         <f>4*5</f>
@@ -4518,7 +4518,7 @@
     </row>
     <row r="22" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B22" s="15">
         <f>4.143*5</f>
@@ -4560,7 +4560,7 @@
     </row>
     <row r="23" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B23" s="7">
         <f>3.82*5</f>
@@ -4601,7 +4601,7 @@
     </row>
     <row r="24" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24" s="7">
         <f>3.45*5</f>
@@ -4658,7 +4658,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="9">
         <v>0</v>
@@ -4693,7 +4693,7 @@
     </row>
     <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="9">
         <f>5*1.58</f>
@@ -4734,7 +4734,7 @@
     </row>
     <row r="3" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="9">
         <f>5*2.15</f>
@@ -4773,7 +4773,7 @@
     </row>
     <row r="4" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="9">
         <f>5*2.7</f>
@@ -4814,7 +4814,7 @@
     </row>
     <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="9">
         <f>5*2.5</f>
@@ -4856,7 +4856,7 @@
     </row>
     <row r="6" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="9">
         <f>5*2.26</f>
@@ -4898,7 +4898,7 @@
     </row>
     <row r="7" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="9">
         <f>5*0.25</f>
@@ -4935,7 +4935,7 @@
     </row>
     <row r="8" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="9">
         <f>5*0.57</f>
@@ -4976,7 +4976,7 @@
     </row>
     <row r="9" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="9">
         <f>5*2.39</f>
@@ -5017,7 +5017,7 @@
     </row>
     <row r="10" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="9">
         <f>5*2.46</f>
@@ -5058,7 +5058,7 @@
     </row>
     <row r="11" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="9">
         <f>5*1.1</f>
@@ -5099,7 +5099,7 @@
     </row>
     <row r="12" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="9">
         <f>5*2.34</f>
@@ -5140,7 +5140,7 @@
     </row>
     <row r="13" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" s="9">
         <f>5*2.6</f>
@@ -5182,7 +5182,7 @@
     </row>
     <row r="14" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="9">
         <f>5*2.76</f>
@@ -5224,7 +5224,7 @@
     </row>
     <row r="15" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" s="9">
         <f>5*2.81</f>
@@ -5265,7 +5265,7 @@
     </row>
     <row r="16" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" s="9">
         <f>5*3.58</f>
@@ -5307,7 +5307,7 @@
     </row>
     <row r="17" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" s="9">
         <f>5*3.06</f>
@@ -5348,7 +5348,7 @@
     </row>
     <row r="18" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18" s="9">
         <f>5*2.3</f>
@@ -5390,7 +5390,7 @@
     </row>
     <row r="19" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B19" s="9">
         <f>5*2.32</f>
@@ -5431,7 +5431,7 @@
     </row>
     <row r="20" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B20" s="22">
         <f t="shared" ref="B20:B21" si="1">5*2</f>
@@ -5472,7 +5472,7 @@
     </row>
     <row r="21" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B21" s="9">
         <f t="shared" si="1"/>
@@ -5513,7 +5513,7 @@
     </row>
     <row r="22" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B22" s="9">
         <f>5*2.29</f>
@@ -5554,7 +5554,7 @@
     </row>
     <row r="23" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B23" s="9">
         <f>5*2.48</f>
@@ -5594,7 +5594,7 @@
     </row>
     <row r="24" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24" s="9">
         <v>11.5</v>
@@ -5649,7 +5649,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="23">
         <v>0</v>
@@ -5676,7 +5676,7 @@
     </row>
     <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="25">
         <v>165.63030000000001</v>
@@ -5703,7 +5703,7 @@
     </row>
     <row r="3" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="25">
         <v>30.4117</v>
@@ -5730,7 +5730,7 @@
     </row>
     <row r="4" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="23">
         <v>0</v>
@@ -5757,7 +5757,7 @@
     </row>
     <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="25">
         <v>12.248100000000001</v>
@@ -5784,7 +5784,7 @@
     </row>
     <row r="6" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="23">
         <v>0</v>
@@ -5811,7 +5811,7 @@
     </row>
     <row r="7" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="23">
         <v>0</v>
@@ -5838,7 +5838,7 @@
     </row>
     <row r="8" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="23">
         <v>0</v>
@@ -5865,7 +5865,7 @@
     </row>
     <row r="9" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="23">
         <v>0</v>
@@ -5892,7 +5892,7 @@
     </row>
     <row r="10" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="23">
         <v>0</v>
@@ -5919,7 +5919,7 @@
     </row>
     <row r="11" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="23">
         <v>0</v>
@@ -5946,7 +5946,7 @@
     </row>
     <row r="12" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="25">
         <v>35.697400000000002</v>
@@ -5973,7 +5973,7 @@
     </row>
     <row r="13" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" s="25">
         <v>14.9194</v>
@@ -6000,7 +6000,7 @@
     </row>
     <row r="14" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="25">
         <v>4.4951999999999996</v>
@@ -6027,7 +6027,7 @@
     </row>
     <row r="15" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" s="23">
         <v>0</v>
@@ -6054,7 +6054,7 @@
     </row>
     <row r="16" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" s="25">
         <v>16.058499999999999</v>
@@ -6081,7 +6081,7 @@
     </row>
     <row r="17" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" s="23">
         <v>0</v>
@@ -6108,7 +6108,7 @@
     </row>
     <row r="18" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18" s="25">
         <v>19.234400000000001</v>
@@ -6135,7 +6135,7 @@
     </row>
     <row r="19" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B19" s="25">
         <v>6.5155000000000003</v>
@@ -6162,7 +6162,7 @@
     </row>
     <row r="20" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B20" s="25">
         <v>70.665800000000004</v>
@@ -6189,7 +6189,7 @@
     </row>
     <row r="21" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B21" s="25">
         <v>16.5383</v>
@@ -6216,7 +6216,7 @@
     </row>
     <row r="22" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B22" s="25">
         <v>0.67969999999999997</v>
@@ -6243,7 +6243,7 @@
     </row>
     <row r="23" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B23" s="25">
         <v>1.3188</v>
@@ -6270,7 +6270,7 @@
     </row>
     <row r="24" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24" s="25">
         <v>29.225300000000001</v>
@@ -6312,7 +6312,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="15">
         <f>0.54*5</f>
@@ -6337,7 +6337,7 @@
     </row>
     <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="15">
         <f>1.85*5</f>
@@ -6362,7 +6362,7 @@
     </row>
     <row r="3" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="15">
         <f>1.138*5</f>
@@ -6387,7 +6387,7 @@
     </row>
     <row r="4" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="15">
         <f>0.284*5</f>
@@ -6412,7 +6412,7 @@
     </row>
     <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="15">
         <f>0.322*5</f>
@@ -6437,7 +6437,7 @@
     </row>
     <row r="6" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="15">
         <f>1.064*5</f>
@@ -6462,7 +6462,7 @@
     </row>
     <row r="7" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="15">
         <f>1.442*5</f>
@@ -6487,7 +6487,7 @@
     </row>
     <row r="8" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="15">
         <f>0.438*5</f>
@@ -6512,7 +6512,7 @@
     </row>
     <row r="9" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="15">
         <f>0.626*5</f>
@@ -6537,7 +6537,7 @@
     </row>
     <row r="10" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="15">
         <f>1.253*5</f>
@@ -6562,7 +6562,7 @@
     </row>
     <row r="11" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="15">
         <f>0.419*5</f>
@@ -6587,7 +6587,7 @@
     </row>
     <row r="12" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="15">
         <f>1.281*5</f>
@@ -6612,7 +6612,7 @@
     </row>
     <row r="13" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" s="15">
         <f>0.886*5</f>
@@ -6637,7 +6637,7 @@
     </row>
     <row r="14" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="15">
         <f>0.447*5</f>
@@ -6662,7 +6662,7 @@
     </row>
     <row r="15" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" s="15">
         <f>0.386*5</f>
@@ -6687,7 +6687,7 @@
     </row>
     <row r="16" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" s="15">
         <f>0.855*5</f>
@@ -6712,7 +6712,7 @@
     </row>
     <row r="17" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" s="15">
         <f>0.357*5</f>
@@ -6737,7 +6737,7 @@
     </row>
     <row r="18" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18" s="15"/>
       <c r="C18" s="26"/>
@@ -6756,7 +6756,7 @@
     </row>
     <row r="19" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B19" s="15">
         <f>0.297*5</f>
@@ -6781,7 +6781,7 @@
     </row>
     <row r="20" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B20" s="15">
         <f>0.44*5</f>
@@ -6806,7 +6806,7 @@
     </row>
     <row r="21" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B21" s="15">
         <f>0.628*5</f>
@@ -6831,7 +6831,7 @@
     </row>
     <row r="22" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B22" s="15">
         <f>0.825*5</f>
@@ -6856,7 +6856,7 @@
     </row>
     <row r="23" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B23" s="15">
         <f>0.272*5</f>
@@ -6881,7 +6881,7 @@
     </row>
     <row r="24" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24" s="12">
         <v>4.5</v>

</xml_diff>

<commit_message>
gas phase transfer corrections to the model. Still needs pruning
</commit_message>
<xml_diff>
--- a/data/exp_raw/johann_batch_preprocessed.xlsx
+++ b/data/exp_raw/johann_batch_preprocessed.xlsx
@@ -641,10 +641,14 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
@@ -1198,7 +1202,7 @@
   <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2564,7 +2568,7 @@
   <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B6" sqref="B6:O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>